<commit_message>
Clase 14 Junio 2017
</commit_message>
<xml_diff>
--- a/Clase_Anaconda.xlsx
+++ b/Clase_Anaconda.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>Edad</t>
   </si>
@@ -155,12 +155,6 @@
   </si>
   <si>
     <t>Hombre</t>
-  </si>
-  <si>
-    <t>Hembra</t>
-  </si>
-  <si>
-    <t>Macho</t>
   </si>
   <si>
     <t>UNAM</t>
@@ -612,19 +606,19 @@
         <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H2">
         <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J2">
         <v>20.07774787474903</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -647,19 +641,19 @@
         <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3">
         <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J3">
         <v>30.07116843195563</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -682,19 +676,19 @@
         <v>45</v>
       </c>
       <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
         <v>49</v>
-      </c>
-      <c r="H4">
-        <v>56</v>
-      </c>
-      <c r="I4" t="s">
-        <v>51</v>
       </c>
       <c r="J4">
         <v>21.875</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -717,19 +711,19 @@
         <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H5">
         <v>56</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J5">
         <v>21.875</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -752,19 +746,19 @@
         <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6">
         <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J6">
         <v>23.59700420642249</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -787,19 +781,19 @@
         <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H7">
         <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J7">
         <v>20.3125</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -822,19 +816,19 @@
         <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8">
         <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8">
         <v>21.97133585722012</v>
       </c>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -857,19 +851,19 @@
         <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H9">
         <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J9">
         <v>21.484375</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -892,7 +886,7 @@
         <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H10">
         <v>55</v>
@@ -901,7 +895,7 @@
         <v>21.484375</v>
       </c>
       <c r="K10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -924,19 +918,19 @@
         <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H11">
         <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J11">
         <v>22.12973972783723</v>
       </c>
       <c r="K11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -959,19 +953,19 @@
         <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H12">
         <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J12">
         <v>19.921875</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -991,22 +985,22 @@
         <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H13">
         <v>60</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J13">
-        <v>25.96952908587257</v>
+        <v>25.96952908587258</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1029,19 +1023,19 @@
         <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H14">
         <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J14">
         <v>26.47210743801653</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1064,19 +1058,19 @@
         <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H15">
         <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J15">
         <v>22.49134948096886</v>
       </c>
       <c r="K15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1096,22 +1090,22 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H16">
         <v>104</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J16">
         <v>32.09876543209877</v>
       </c>
       <c r="K16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>